<commit_message>
set exact match comaprison for gap common pair v3
</commit_message>
<xml_diff>
--- a/swertres/digit_position.xlsx
+++ b/swertres/digit_position.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00720558"/>
+        <fgColor rgb="00705170"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00712347"/>
+        <fgColor rgb="00736235"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00770557"/>
+        <fgColor rgb="00736142"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00756774"/>
+        <fgColor rgb="00728258"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00763334"/>
+        <fgColor rgb="00737416"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00743486"/>
+        <fgColor rgb="00753980"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00755644"/>
+        <fgColor rgb="00747609"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00723137"/>
+        <fgColor rgb="00748877"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00718931"/>
+        <fgColor rgb="00743491"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00776363"/>
+        <fgColor rgb="00716500"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>